<commit_message>
states to target for EV
</commit_message>
<xml_diff>
--- a/Datasets/Geographic Data/type_AP.xlsx
+++ b/Datasets/Geographic Data/type_AP.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\EV-Market-Segmentation\Datasets\Geographic Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11952" windowHeight="5064"/>
   </bookViews>
   <sheets>
-    <sheet name="reportTable" r:id="rId3" sheetId="1"/>
+    <sheet name="reportTable" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="246">
   <si>
     <t>Vehicle Class Wise Fuel Data  of Andhra Pradesh ( Till Today )</t>
   </si>
@@ -755,24 +762,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Calibri"/>
-      <sz val="10.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="8.0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -780,7 +782,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -795,96 +797,402 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:X64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.37890625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="36.55078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.65625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="9.20703125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="15.09765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.7109375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="21.625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="17.80078125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="17.54296875" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="15.26171875" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="9.79296875" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="21.84375" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="4.859375" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="10.12890625" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="11.37109375" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="16.55859375" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" width="10.375" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" width="12.85546875" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" width="17.53125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.765625" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="12.33203125" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="19.11328125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="7.19921875" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="10.375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="5">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="X2" t="s" s="5">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3">
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="1"/>
+      <c r="X3" s="3"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
@@ -952,7 +1260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1026,7 +1334,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1100,7 +1408,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1174,7 +1482,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1248,7 +1556,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1322,7 +1630,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1396,7 +1704,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -1470,7 +1778,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1544,7 +1852,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -1618,7 +1926,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1692,7 +2000,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -1766,7 +2074,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -1840,7 +2148,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1914,7 +2222,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1988,7 +2296,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>91</v>
       </c>
@@ -2062,7 +2370,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -2136,7 +2444,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>96</v>
       </c>
@@ -2210,7 +2518,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -2284,7 +2592,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -2358,7 +2666,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -2432,7 +2740,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -2506,7 +2814,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>66</v>
       </c>
@@ -2580,7 +2888,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -2654,7 +2962,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>124</v>
       </c>
@@ -2728,7 +3036,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>103</v>
       </c>
@@ -2802,7 +3110,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>104</v>
       </c>
@@ -2876,7 +3184,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>128</v>
       </c>
@@ -2950,7 +3258,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>131</v>
       </c>
@@ -3024,7 +3332,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -3098,7 +3406,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -3172,7 +3480,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -3246,7 +3554,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>151</v>
       </c>
@@ -3320,7 +3628,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>153</v>
       </c>
@@ -3394,7 +3702,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>158</v>
       </c>
@@ -3468,7 +3776,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>166</v>
       </c>
@@ -3542,7 +3850,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -3616,7 +3924,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>181</v>
       </c>
@@ -3690,7 +3998,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>188</v>
       </c>
@@ -3764,7 +4072,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>190</v>
       </c>
@@ -3838,7 +4146,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>195</v>
       </c>
@@ -3912,7 +4220,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>133</v>
       </c>
@@ -3986,7 +4294,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>201</v>
       </c>
@@ -4060,7 +4368,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>70</v>
       </c>
@@ -4134,7 +4442,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>155</v>
       </c>
@@ -4208,7 +4516,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>214</v>
       </c>
@@ -4282,7 +4590,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>71</v>
       </c>
@@ -4356,7 +4664,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>77</v>
       </c>
@@ -4430,7 +4738,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>218</v>
       </c>
@@ -4504,7 +4812,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>224</v>
       </c>
@@ -4578,7 +4886,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>229</v>
       </c>
@@ -4652,7 +4960,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>89</v>
       </c>
@@ -4726,7 +5034,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>236</v>
       </c>
@@ -4800,7 +5108,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>238</v>
       </c>
@@ -4874,7 +5182,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>240</v>
       </c>
@@ -4948,7 +5256,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>242</v>
       </c>
@@ -5022,7 +5330,6 @@
         <v>245</v>
       </c>
     </row>
-    <row r="64"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:X1"/>
@@ -5031,8 +5338,8 @@
     <mergeCell ref="C2:W2"/>
     <mergeCell ref="X2:X3"/>
   </mergeCells>
-  <printOptions gridLines="true"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape" paperSize="9"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
 </worksheet>
 </file>
</xml_diff>